<commit_message>
added test for calcrule 19 and updates for calcrule 25 change
</commit_message>
<xml_diff>
--- a/ftest/data/fm35/Worked example policy calculation_PcntLossMinandMaxdeductibles.xlsx
+++ b/ftest/data/fm35/Worked example policy calculation_PcntLossMinandMaxdeductibles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3C820010-7499-4893-8E6C-CA6F2EB1DF6E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5576FDE9-BA7B-4775-AFBE-8196BE423FD1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="sidx 2" sheetId="11" r:id="rId2"/>
     <sheet name="sidx 3" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -562,19 +562,19 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1019,8 +1019,8 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1509,14 +1509,14 @@
       <c r="B25" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
       <c r="K25" s="44"/>
       <c r="L25" s="52">
         <f>L22+L23-L24</f>
@@ -1799,13 +1799,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:J25"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C20:J20"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="C22:J22"/>
     <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
@@ -1820,7 +1820,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:J16"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1849,8 +1849,8 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -2339,14 +2339,14 @@
       <c r="B25" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
       <c r="K25" s="44"/>
       <c r="L25" s="52">
         <f>L22+L23-L24</f>
@@ -2629,13 +2629,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:J25"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C20:J20"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="C22:J22"/>
     <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
@@ -2650,7 +2650,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2679,8 +2679,8 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -3169,14 +3169,14 @@
       <c r="B25" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
       <c r="K25" s="44"/>
       <c r="L25" s="52">
         <f>L22+L23-L24</f>

</xml_diff>